<commit_message>
[27/08/23] Rename amol to policyBazar
</commit_message>
<xml_diff>
--- a/TestData/SeleniumRevisionC'wad.xlsx
+++ b/TestData/SeleniumRevisionC'wad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shree\git\SeleniumRevisionMaven1\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shree\eclipse-workspace\For_Amol_\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898C4C5F-9182-44E7-8FB9-D88A1A582D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E9C9C6-8C59-484E-A83A-50F7D4F33D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="1785" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>abc</t>
   </si>
@@ -59,13 +59,16 @@
     <t>pdkqwd</t>
   </si>
   <si>
-    <t>Jan batch</t>
-  </si>
-  <si>
     <t>7020500587</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
+    <t>abcd@1234</t>
+  </si>
+  <si>
+    <t>Harshal Patil</t>
+  </si>
+  <si>
+    <t>658192396</t>
   </si>
 </sst>
 </file>
@@ -116,12 +119,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -520,35 +522,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668692A-5649-4473-B42D-EA9DE28AA914}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{4FCD1CFC-F5E6-47E5-AC6E-9CE2B3C2B91B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3D103D52-8B6E-4B69-8B99-36DDD074CB04}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>